<commit_message>
add genders in batumi
</commit_message>
<xml_diff>
--- a/municipal/ENG/Education/General Educational Institution/Guria/Lanchkhuti.xlsx
+++ b/municipal/ENG/Education/General Educational Institution/Guria/Lanchkhuti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tgrigolishvili\Desktop\სკოლები\General Educational Institution\Guria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamashukeli\Desktop\General Educational Institution\Guria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2515D02-84DD-4677-824A-104EB6507550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5462FF-0BFD-4DB4-B3DA-C34CF1ECF5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="795" windowWidth="20850" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lanchkhuti" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t>Public and Private General Education Schools in Lanchkhuti municipality</t>
   </si>
@@ -125,14 +125,20 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>number of graduates of the primary level (persons)</t>
+  </si>
+  <si>
+    <t>number of graduates of the basic level (persons)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="#\ ##0"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="#\ ##0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -168,23 +174,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -204,6 +193,23 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -261,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -271,49 +277,47 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -619,516 +623,798 @@
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" ht="21" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="18" t="s">
+      <c r="O3" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="21" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="10">
         <v>25</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="10">
         <v>25</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="10">
         <v>25</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="10">
         <v>25</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="10">
         <v>25</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="10">
         <v>25</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="10">
         <v>25</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="10">
         <v>25</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="10">
         <v>25</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="10">
         <v>25</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="10">
         <v>25</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="10">
         <v>25</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="10">
         <v>25</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="10">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="21" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="11">
         <v>4533</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="12">
         <v>4243</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="12">
         <v>4124</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="12">
         <v>3935</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="12">
         <v>3779</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="12">
         <v>3719</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="12">
         <v>3762</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="12">
         <v>3731</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="12">
         <v>3655</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="12">
         <v>3636</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="12">
         <v>3645</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="12">
         <v>3717</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="12">
         <v>3716</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="11">
         <v>3666</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="30">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:18" ht="26.25">
+      <c r="A6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="12">
+        <v>373</v>
+      </c>
+      <c r="D6" s="12">
+        <v>294</v>
+      </c>
+      <c r="E6" s="12">
+        <v>346</v>
+      </c>
+      <c r="F6" s="12">
+        <v>333</v>
+      </c>
+      <c r="G6" s="12">
+        <v>306</v>
+      </c>
+      <c r="H6" s="12">
+        <v>309</v>
+      </c>
+      <c r="I6" s="12">
+        <v>297</v>
+      </c>
+      <c r="J6" s="12">
+        <v>253</v>
+      </c>
+      <c r="K6" s="12">
+        <v>260</v>
+      </c>
+      <c r="L6" s="12">
+        <v>290</v>
+      </c>
+      <c r="M6" s="12">
+        <v>365</v>
+      </c>
+      <c r="N6" s="12">
+        <v>358</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="12">
+        <v>184</v>
+      </c>
+      <c r="D7" s="12">
+        <v>138</v>
+      </c>
+      <c r="E7" s="12">
+        <v>162</v>
+      </c>
+      <c r="F7" s="12">
+        <v>153</v>
+      </c>
+      <c r="G7" s="12">
+        <v>149</v>
+      </c>
+      <c r="H7" s="12">
+        <v>162</v>
+      </c>
+      <c r="I7" s="12">
+        <v>125</v>
+      </c>
+      <c r="J7" s="12">
+        <v>127</v>
+      </c>
+      <c r="K7" s="12">
+        <v>122</v>
+      </c>
+      <c r="L7" s="12">
+        <v>138</v>
+      </c>
+      <c r="M7" s="12">
+        <v>167</v>
+      </c>
+      <c r="N7" s="12">
+        <v>183</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="12">
+        <v>189</v>
+      </c>
+      <c r="D8" s="12">
+        <v>156</v>
+      </c>
+      <c r="E8" s="12">
+        <v>184</v>
+      </c>
+      <c r="F8" s="12">
+        <v>180</v>
+      </c>
+      <c r="G8" s="12">
+        <v>157</v>
+      </c>
+      <c r="H8" s="12">
+        <v>147</v>
+      </c>
+      <c r="I8" s="12">
+        <v>172</v>
+      </c>
+      <c r="J8" s="12">
+        <v>126</v>
+      </c>
+      <c r="K8" s="12">
+        <v>138</v>
+      </c>
+      <c r="L8" s="12">
+        <v>152</v>
+      </c>
+      <c r="M8" s="12">
+        <v>198</v>
+      </c>
+      <c r="N8" s="12">
+        <v>175</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="26.25">
+      <c r="A9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="12">
+        <v>417</v>
+      </c>
+      <c r="D9" s="12">
+        <v>408</v>
+      </c>
+      <c r="E9" s="12">
+        <v>366</v>
+      </c>
+      <c r="F9" s="12">
+        <v>373</v>
+      </c>
+      <c r="G9" s="12">
+        <v>306</v>
+      </c>
+      <c r="H9" s="12">
+        <v>343</v>
+      </c>
+      <c r="I9" s="12">
+        <v>309</v>
+      </c>
+      <c r="J9" s="12">
+        <v>306</v>
+      </c>
+      <c r="K9" s="12">
+        <v>299</v>
+      </c>
+      <c r="L9" s="12">
+        <v>296</v>
+      </c>
+      <c r="M9" s="12">
+        <v>250</v>
+      </c>
+      <c r="N9" s="12">
+        <v>256</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="12">
+        <v>209</v>
+      </c>
+      <c r="D10" s="12">
+        <v>169</v>
+      </c>
+      <c r="E10" s="12">
+        <v>185</v>
+      </c>
+      <c r="F10" s="12">
+        <v>191</v>
+      </c>
+      <c r="G10" s="12">
+        <v>141</v>
+      </c>
+      <c r="H10" s="12">
+        <v>162</v>
+      </c>
+      <c r="I10" s="12">
+        <v>144</v>
+      </c>
+      <c r="J10" s="12">
+        <v>146</v>
+      </c>
+      <c r="K10" s="12">
+        <v>160</v>
+      </c>
+      <c r="L10" s="12">
+        <v>126</v>
+      </c>
+      <c r="M10" s="12">
+        <v>123</v>
+      </c>
+      <c r="N10" s="12">
+        <v>114</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="12">
+        <v>208</v>
+      </c>
+      <c r="D11" s="12">
+        <v>239</v>
+      </c>
+      <c r="E11" s="12">
+        <v>181</v>
+      </c>
+      <c r="F11" s="12">
+        <v>182</v>
+      </c>
+      <c r="G11" s="12">
+        <v>165</v>
+      </c>
+      <c r="H11" s="12">
+        <v>181</v>
+      </c>
+      <c r="I11" s="12">
+        <v>165</v>
+      </c>
+      <c r="J11" s="12">
+        <v>160</v>
+      </c>
+      <c r="K11" s="12">
+        <v>139</v>
+      </c>
+      <c r="L11" s="12">
+        <v>170</v>
+      </c>
+      <c r="M11" s="12">
+        <v>127</v>
+      </c>
+      <c r="N11" s="12">
+        <v>142</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="26.25">
+      <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="13">
-        <v>302</v>
-      </c>
-      <c r="D6" s="13">
-        <v>289</v>
-      </c>
-      <c r="E6" s="13">
-        <v>308</v>
-      </c>
-      <c r="F6" s="13">
-        <v>293</v>
-      </c>
-      <c r="G6" s="13">
-        <v>270</v>
-      </c>
-      <c r="H6" s="13">
-        <v>282</v>
-      </c>
-      <c r="I6" s="13">
+      <c r="B12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="12">
+        <v>307</v>
+      </c>
+      <c r="D12" s="12">
+        <v>317</v>
+      </c>
+      <c r="E12" s="12">
+        <v>306</v>
+      </c>
+      <c r="F12" s="12">
+        <v>283</v>
+      </c>
+      <c r="G12" s="12">
+        <v>288</v>
+      </c>
+      <c r="H12" s="12">
+        <v>301</v>
+      </c>
+      <c r="I12" s="12">
         <v>309</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J12" s="12">
         <v>252</v>
       </c>
-      <c r="K6" s="13">
-        <v>302</v>
-      </c>
-      <c r="L6" s="13">
+      <c r="K12" s="12">
+        <v>298</v>
+      </c>
+      <c r="L12" s="12">
         <v>266</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M12" s="12">
         <v>288</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N12" s="12">
         <v>304</v>
       </c>
-      <c r="O6" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="21" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="O12" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="21" customHeight="1">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="11">
-        <v>170</v>
-      </c>
-      <c r="D7" s="11">
-        <v>151</v>
-      </c>
-      <c r="E7" s="11">
-        <v>164</v>
-      </c>
-      <c r="F7" s="11">
+      <c r="B13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="12">
+        <v>175</v>
+      </c>
+      <c r="D13" s="12">
+        <v>162</v>
+      </c>
+      <c r="E13" s="12">
+        <v>163</v>
+      </c>
+      <c r="F13" s="12">
+        <v>152</v>
+      </c>
+      <c r="G13" s="12">
+        <v>134</v>
+      </c>
+      <c r="H13" s="12">
+        <v>149</v>
+      </c>
+      <c r="I13" s="12">
+        <v>168</v>
+      </c>
+      <c r="J13" s="12">
+        <v>126</v>
+      </c>
+      <c r="K13" s="12">
+        <v>140</v>
+      </c>
+      <c r="L13" s="12">
+        <v>127</v>
+      </c>
+      <c r="M13" s="12">
+        <v>142</v>
+      </c>
+      <c r="N13" s="12">
+        <v>161</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="21" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="12">
+        <v>132</v>
+      </c>
+      <c r="D14" s="12">
+        <v>155</v>
+      </c>
+      <c r="E14" s="12">
+        <v>143</v>
+      </c>
+      <c r="F14" s="12">
+        <v>131</v>
+      </c>
+      <c r="G14" s="12">
         <v>154</v>
       </c>
-      <c r="G7" s="11">
-        <v>127</v>
-      </c>
-      <c r="H7" s="11">
-        <v>145</v>
-      </c>
-      <c r="I7" s="11">
-        <v>168</v>
-      </c>
-      <c r="J7" s="11">
-        <v>136</v>
-      </c>
-      <c r="K7" s="11">
+      <c r="H14" s="12">
+        <v>152</v>
+      </c>
+      <c r="I14" s="12">
+        <v>141</v>
+      </c>
+      <c r="J14" s="12">
+        <v>126</v>
+      </c>
+      <c r="K14" s="12">
+        <v>158</v>
+      </c>
+      <c r="L14" s="12">
+        <v>139</v>
+      </c>
+      <c r="M14" s="12">
+        <v>146</v>
+      </c>
+      <c r="N14" s="12">
         <v>143</v>
       </c>
-      <c r="L7" s="11">
-        <v>127</v>
-      </c>
-      <c r="M7" s="11">
-        <v>142</v>
-      </c>
-      <c r="N7" s="11">
-        <v>161</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="21" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="11">
-        <v>132</v>
-      </c>
-      <c r="D8" s="11">
-        <v>138</v>
-      </c>
-      <c r="E8" s="11">
-        <v>144</v>
-      </c>
-      <c r="F8" s="11">
-        <v>139</v>
-      </c>
-      <c r="G8" s="11">
-        <v>143</v>
-      </c>
-      <c r="H8" s="11">
-        <v>137</v>
-      </c>
-      <c r="I8" s="11">
-        <v>141</v>
-      </c>
-      <c r="J8" s="11">
-        <v>126</v>
-      </c>
-      <c r="K8" s="11">
-        <v>159</v>
-      </c>
-      <c r="L8" s="11">
-        <v>139</v>
-      </c>
-      <c r="M8" s="11">
-        <v>145</v>
-      </c>
-      <c r="N8" s="11">
-        <v>143</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="26.25">
-      <c r="A9" s="14" t="s">
+      <c r="O14" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="26.25">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="22">
-        <v>9.2895922730278802</v>
-      </c>
-      <c r="D9" s="22">
-        <v>8.9483380552072198</v>
-      </c>
-      <c r="E9" s="22">
-        <v>9.6144841579522407</v>
-      </c>
-      <c r="F9" s="22">
-        <v>9.2144160010063505</v>
-      </c>
-      <c r="G9" s="22">
-        <v>8.5470085470085504</v>
-      </c>
-      <c r="H9" s="22">
-        <v>8.9774608429899398</v>
-      </c>
-      <c r="I9" s="22">
-        <v>9.9051160405180205</v>
-      </c>
-      <c r="J9" s="22">
-        <v>8.1466395112016308</v>
-      </c>
-      <c r="K9" s="22">
-        <v>9.8523774569774094</v>
-      </c>
-      <c r="L9" s="22">
-        <v>8.7712067004105307</v>
-      </c>
-      <c r="M9" s="22">
-        <v>9.5928053959530306</v>
-      </c>
-      <c r="N9" s="22">
-        <v>10.3805637602226</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="21" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="B15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="20">
+        <v>9.5056739894415827</v>
+      </c>
+      <c r="D15" s="20">
+        <v>9.8954268768534419</v>
+      </c>
+      <c r="E15" s="20">
+        <v>9.6232467450783066</v>
+      </c>
+      <c r="F15" s="20">
+        <v>8.9585311807534023</v>
+      </c>
+      <c r="G15" s="20">
+        <v>9.1684706481599392</v>
+      </c>
+      <c r="H15" s="20">
+        <v>9.6486729067829202</v>
+      </c>
+      <c r="I15" s="20">
+        <v>9.9893317815924743</v>
+      </c>
+      <c r="J15" s="20">
+        <v>8.2211891362857834</v>
+      </c>
+      <c r="K15" s="20">
+        <v>9.8263894613621758</v>
+      </c>
+      <c r="L15" s="20">
+        <v>8.8600216504288447</v>
+      </c>
+      <c r="M15" s="20">
+        <v>9.711029436557979</v>
+      </c>
+      <c r="N15" s="20">
+        <v>10.380563760222635</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="21" customHeight="1">
+      <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="11">
+      <c r="B16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="12">
         <v>665</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I16" s="12">
         <v>675</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J16" s="12">
         <v>654</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K16" s="12">
         <v>604</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L16" s="12">
         <v>582</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M16" s="12">
         <v>551</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N16" s="12">
         <v>577</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O16" s="12">
         <v>575</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="21" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="17" spans="1:15" ht="21" customHeight="1">
+      <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="11">
+      <c r="B17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="12">
         <v>546</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I17" s="12">
         <v>557</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J17" s="12">
         <v>539</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K17" s="12">
         <v>492</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L17" s="12">
         <v>481</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M17" s="12">
         <v>457</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N17" s="12">
         <v>484</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O17" s="12">
         <v>476</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="21" customHeight="1">
-      <c r="A12" s="15" t="s">
+    <row r="18" spans="1:15" ht="21" customHeight="1">
+      <c r="A18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="16">
+      <c r="B18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="13">
         <v>119</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I18" s="13">
         <v>118</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J18" s="13">
         <v>115</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K18" s="13">
         <v>112</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L18" s="13">
         <v>101</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M18" s="13">
         <v>94</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N18" s="13">
         <v>93</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O18" s="13">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="20" t="s">
+    <row r="19" spans="1:15">
+      <c r="A19" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-    </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1">
-      <c r="A14" s="21" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1">
+      <c r="A20" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>